<commit_message>
Weighting Scripts Stage 2
</commit_message>
<xml_diff>
--- a/02_MasterWifoMannheim/04_Graph/CourseSkillWeights_Master.xlsx
+++ b/02_MasterWifoMannheim/04_Graph/CourseSkillWeights_Master.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mailunimannheimde-my.sharepoint.com/personal/pstapf_mail_uni-mannheim_de/Documents/Uni/Master/Masterarbeit/Course_Suggestion/02_MasterWifoMannheim/04_Graph/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="11_113D30A1D3B05E4B2F783611595ED87656CC33C8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0870EA0A-5200-4827-A12A-8ECD54593281}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="11_329513BED3A0DE491B1A2E11595ED87656CC70CA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FF48F5B5-010C-4B53-A68F-ACF78E3CA6EA}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-25245" yWindow="1215" windowWidth="21600" windowHeight="14070" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -992,10 +992,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:E273"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A226" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:A273"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1017,9 +1018,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>1.4668319735509101</v>
+        <v>1.2272770054051141</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
@@ -1028,15 +1029,15 @@
         <v>6</v>
       </c>
       <c r="D2">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="E2">
-        <v>912</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>907</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>85.009238549061536</v>
+        <v>84.409340659340671</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
@@ -1048,12 +1049,12 @@
         <v>91</v>
       </c>
       <c r="E3">
-        <v>1469</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1456</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>74.488421550094529</v>
+        <v>73.460714285714289</v>
       </c>
       <c r="B4" t="s">
         <v>9</v>
@@ -1065,12 +1066,12 @@
         <v>80</v>
       </c>
       <c r="E4">
-        <v>2116</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>2100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>73.434299754299786</v>
+        <v>72.828789141564471</v>
       </c>
       <c r="B5" t="s">
         <v>11</v>
@@ -1082,12 +1083,12 @@
         <v>185</v>
       </c>
       <c r="E5">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1362</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>10.908985251217469</v>
+        <v>7.7866806153261052</v>
       </c>
       <c r="B6" t="s">
         <v>12</v>
@@ -1096,15 +1097,15 @@
         <v>13</v>
       </c>
       <c r="D6">
-        <v>619</v>
+        <v>614</v>
       </c>
       <c r="E6">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B7" t="s">
         <v>12</v>
@@ -1113,15 +1114,15 @@
         <v>14</v>
       </c>
       <c r="D7">
-        <v>1386</v>
+        <v>1376</v>
       </c>
       <c r="E7">
-        <v>2067</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <v>2050</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>25.338962243561749</v>
+        <v>24.793842313293109</v>
       </c>
       <c r="B8" t="s">
         <v>12</v>
@@ -1130,15 +1131,15 @@
         <v>8</v>
       </c>
       <c r="D8">
-        <v>928</v>
+        <v>920</v>
       </c>
       <c r="E8">
-        <v>632</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>64.195501730103786</v>
+        <v>63.916317250339567</v>
       </c>
       <c r="B9" t="s">
         <v>15</v>
@@ -1147,15 +1148,15 @@
         <v>13</v>
       </c>
       <c r="D9">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="E9">
-        <v>578</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>22.08285714285714</v>
+        <v>21.698784805281779</v>
       </c>
       <c r="B10" t="s">
         <v>16</v>
@@ -1167,12 +1168,12 @@
         <v>70</v>
       </c>
       <c r="E10">
-        <v>1500</v>
+        <v>1493</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B11" t="s">
         <v>17</v>
@@ -1187,9 +1188,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>186.27296587926509</v>
+        <v>186.01583113456459</v>
       </c>
       <c r="B12" t="s">
         <v>17</v>
@@ -1201,12 +1202,12 @@
         <v>1</v>
       </c>
       <c r="E12">
-        <v>381</v>
+        <v>379</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B13" t="s">
         <v>20</v>
@@ -1218,12 +1219,12 @@
         <v>12</v>
       </c>
       <c r="E13">
-        <v>746</v>
+        <v>739</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B14" t="s">
         <v>20</v>
@@ -1240,7 +1241,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B15" t="s">
         <v>22</v>
@@ -1252,12 +1253,12 @@
         <v>16</v>
       </c>
       <c r="E15">
-        <v>742</v>
+        <v>735</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B16" t="s">
         <v>22</v>
@@ -1272,9 +1273,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>82.495136186770424</v>
+        <v>80.059523809523796</v>
       </c>
       <c r="B17" t="s">
         <v>23</v>
@@ -1286,12 +1287,12 @@
         <v>8</v>
       </c>
       <c r="E17">
-        <v>257</v>
+        <v>252</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B18" t="s">
         <v>23</v>
@@ -1303,12 +1304,12 @@
         <v>20</v>
       </c>
       <c r="E18">
-        <v>2176</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+        <v>2160</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>17.27660285881467</v>
+        <v>16.631419303197561</v>
       </c>
       <c r="B19" t="s">
         <v>23</v>
@@ -1320,12 +1321,12 @@
         <v>35</v>
       </c>
       <c r="E19">
-        <v>3418</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+        <v>3391</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>64.176470588235304</v>
+        <v>61.720000000000027</v>
       </c>
       <c r="B20" t="s">
         <v>25</v>
@@ -1337,12 +1338,12 @@
         <v>10</v>
       </c>
       <c r="E20">
-        <v>255</v>
+        <v>250</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B21" t="s">
         <v>25</v>
@@ -1351,15 +1352,15 @@
         <v>8</v>
       </c>
       <c r="D21">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E21">
-        <v>1460</v>
+        <v>1448</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B22" t="s">
         <v>25</v>
@@ -1371,12 +1372,12 @@
         <v>0</v>
       </c>
       <c r="E22">
-        <v>234</v>
+        <v>229</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B23" t="s">
         <v>27</v>
@@ -1388,12 +1389,12 @@
         <v>0</v>
       </c>
       <c r="E23">
-        <v>265</v>
+        <v>260</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B24" t="s">
         <v>27</v>
@@ -1405,12 +1406,12 @@
         <v>0</v>
       </c>
       <c r="E24">
-        <v>234</v>
+        <v>229</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B25" t="s">
         <v>27</v>
@@ -1422,12 +1423,12 @@
         <v>0</v>
       </c>
       <c r="E25">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>60.328221592267482</v>
+        <v>59.720653072471748</v>
       </c>
       <c r="B26" t="s">
         <v>29</v>
@@ -1439,12 +1440,12 @@
         <v>19</v>
       </c>
       <c r="E26">
-        <v>1541</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1528</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>12.741966705381291</v>
+        <v>12.10697197539298</v>
       </c>
       <c r="B27" t="s">
         <v>30</v>
@@ -1456,12 +1457,12 @@
         <v>84</v>
       </c>
       <c r="E27">
-        <v>1476</v>
+        <v>1463</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B28" t="s">
         <v>30</v>
@@ -1473,12 +1474,12 @@
         <v>52</v>
       </c>
       <c r="E28">
-        <v>706</v>
+        <v>699</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B29" t="s">
         <v>30</v>
@@ -1490,12 +1491,12 @@
         <v>8</v>
       </c>
       <c r="E29">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>18.52535472305777</v>
+        <v>19.626859916297349</v>
       </c>
       <c r="B30" t="s">
         <v>31</v>
@@ -1504,15 +1505,15 @@
         <v>8</v>
       </c>
       <c r="D30">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="E30">
-        <v>1242</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1231</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>9.8884321785085092</v>
+        <v>9.6012498140157732</v>
       </c>
       <c r="B31" t="s">
         <v>31</v>
@@ -1524,12 +1525,12 @@
         <v>234</v>
       </c>
       <c r="E31">
-        <v>524</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>36.487933634992459</v>
+        <v>36.27462186154608</v>
       </c>
       <c r="B32" t="s">
         <v>32</v>
@@ -1541,12 +1542,12 @@
         <v>78</v>
       </c>
       <c r="E32">
-        <v>680</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>1.9362455726092089</v>
+        <v>2.3928571428571388</v>
       </c>
       <c r="B33" t="s">
         <v>32</v>
@@ -1558,12 +1559,12 @@
         <v>35</v>
       </c>
       <c r="E33">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>28.574374079528749</v>
+        <v>27.941285251964871</v>
       </c>
       <c r="B34" t="s">
         <v>32</v>
@@ -1575,12 +1576,12 @@
         <v>105</v>
       </c>
       <c r="E34">
-        <v>1455</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1442</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>12.29666719652414</v>
+        <v>10.629280821917799</v>
       </c>
       <c r="B35" t="s">
         <v>33</v>
@@ -1589,15 +1590,15 @@
         <v>8</v>
       </c>
       <c r="D35">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E35">
-        <v>1398</v>
+        <v>1387</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B36" t="s">
         <v>33</v>
@@ -1609,12 +1610,12 @@
         <v>27</v>
       </c>
       <c r="E36">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>17.531686707832279</v>
+        <v>17.302485847895639</v>
       </c>
       <c r="B37" t="s">
         <v>34</v>
@@ -1626,12 +1627,12 @@
         <v>34</v>
       </c>
       <c r="E37">
-        <v>724</v>
+        <v>717</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B38" t="s">
         <v>34</v>
@@ -1643,12 +1644,12 @@
         <v>64</v>
       </c>
       <c r="E38">
-        <v>1496</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1483</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>18.38244514106583</v>
+        <v>18.76893939393938</v>
       </c>
       <c r="B39" t="s">
         <v>34</v>
@@ -1660,12 +1661,12 @@
         <v>11</v>
       </c>
       <c r="E39">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>12.095055413469741</v>
+        <v>10.4793187347932</v>
       </c>
       <c r="B40" t="s">
         <v>35</v>
@@ -1674,15 +1675,15 @@
         <v>13</v>
       </c>
       <c r="D40">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E40">
-        <v>690</v>
+        <v>685</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B41" t="s">
         <v>35</v>
@@ -1691,15 +1692,15 @@
         <v>14</v>
       </c>
       <c r="D41">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="E41">
-        <v>3239</v>
+        <v>3216</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B42" t="s">
         <v>35</v>
@@ -1708,15 +1709,15 @@
         <v>8</v>
       </c>
       <c r="D42">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="E42">
-        <v>1441</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1431</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>66.326203208556137</v>
+        <v>66.10526315789474</v>
       </c>
       <c r="B43" t="s">
         <v>36</v>
@@ -1728,12 +1729,12 @@
         <v>10</v>
       </c>
       <c r="E43">
-        <v>748</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+        <v>741</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>49.785214785214777</v>
+        <v>49.143696245017821</v>
       </c>
       <c r="B44" t="s">
         <v>37</v>
@@ -1745,12 +1746,12 @@
         <v>21</v>
       </c>
       <c r="E44">
-        <v>3432</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+        <v>3405</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45">
-        <v>39.366666666666667</v>
+        <v>39.141991924629878</v>
       </c>
       <c r="B45" t="s">
         <v>37</v>
@@ -1762,12 +1763,12 @@
         <v>8</v>
       </c>
       <c r="E45">
-        <v>750</v>
+        <v>743</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B46" t="s">
         <v>38</v>
@@ -1779,12 +1780,12 @@
         <v>1</v>
       </c>
       <c r="E46">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B47" t="s">
         <v>38</v>
@@ -1799,9 +1800,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48">
-        <v>35.009404388714728</v>
+        <v>35.404040404040423</v>
       </c>
       <c r="B48" t="s">
         <v>41</v>
@@ -1813,12 +1814,12 @@
         <v>11</v>
       </c>
       <c r="E48">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49">
-        <v>5.1407989521938484</v>
+        <v>4.5222369000439926</v>
       </c>
       <c r="B49" t="s">
         <v>41</v>
@@ -1830,12 +1831,12 @@
         <v>33</v>
       </c>
       <c r="E49">
-        <v>1527</v>
+        <v>1514</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B50" t="s">
         <v>41</v>
@@ -1847,12 +1848,12 @@
         <v>30</v>
       </c>
       <c r="E50">
-        <v>728</v>
+        <v>721</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B51" t="s">
         <v>42</v>
@@ -1864,12 +1865,12 @@
         <v>83</v>
       </c>
       <c r="E51">
-        <v>1477</v>
+        <v>1464</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B52" t="s">
         <v>42</v>
@@ -1881,12 +1882,12 @@
         <v>18</v>
       </c>
       <c r="E52">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B53" t="s">
         <v>43</v>
@@ -1898,12 +1899,12 @@
         <v>18</v>
       </c>
       <c r="E53">
-        <v>740</v>
+        <v>733</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B54" t="s">
         <v>43</v>
@@ -1915,12 +1916,12 @@
         <v>25</v>
       </c>
       <c r="E54">
-        <v>1535</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1522</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55">
-        <v>18.039215686274531</v>
+        <v>18.399122807017559</v>
       </c>
       <c r="B55" t="s">
         <v>43</v>
@@ -1932,12 +1933,12 @@
         <v>3</v>
       </c>
       <c r="E55">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B56" t="s">
         <v>44</v>
@@ -1949,12 +1950,12 @@
         <v>2</v>
       </c>
       <c r="E56">
-        <v>756</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+        <v>749</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57">
-        <v>9.150064936656122</v>
+        <v>8.8486177499630401</v>
       </c>
       <c r="B57" t="s">
         <v>45</v>
@@ -1963,7 +1964,7 @@
         <v>46</v>
       </c>
       <c r="D57">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="E57">
         <v>223</v>
@@ -1971,7 +1972,7 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B58" t="s">
         <v>47</v>
@@ -1980,7 +1981,7 @@
         <v>46</v>
       </c>
       <c r="D58">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="E58">
         <v>275</v>
@@ -1988,7 +1989,7 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B59" t="s">
         <v>48</v>
@@ -2000,12 +2001,12 @@
         <v>0</v>
       </c>
       <c r="E59">
-        <v>589</v>
+        <v>587</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B60" t="s">
         <v>48</v>
@@ -2017,12 +2018,12 @@
         <v>0</v>
       </c>
       <c r="E60">
-        <v>265</v>
+        <v>260</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B61" t="s">
         <v>48</v>
@@ -2034,12 +2035,12 @@
         <v>0</v>
       </c>
       <c r="E61">
-        <v>2196</v>
+        <v>2180</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B62" t="s">
         <v>49</v>
@@ -2051,12 +2052,12 @@
         <v>8</v>
       </c>
       <c r="E62">
-        <v>750</v>
+        <v>743</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B63" t="s">
         <v>49</v>
@@ -2068,12 +2069,12 @@
         <v>0</v>
       </c>
       <c r="E63">
-        <v>589</v>
+        <v>587</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B64" t="s">
         <v>50</v>
@@ -2085,12 +2086,12 @@
         <v>0</v>
       </c>
       <c r="E64">
-        <v>589</v>
+        <v>587</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B65" t="s">
         <v>50</v>
@@ -2102,12 +2103,12 @@
         <v>5</v>
       </c>
       <c r="E65">
-        <v>1555</v>
+        <v>1542</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B66" t="s">
         <v>51</v>
@@ -2119,12 +2120,12 @@
         <v>0</v>
       </c>
       <c r="E66">
-        <v>589</v>
+        <v>587</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B67" t="s">
         <v>51</v>
@@ -2133,15 +2134,15 @@
         <v>8</v>
       </c>
       <c r="D67">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E67">
-        <v>1528</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1516</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68">
-        <v>14.175603217158169</v>
+        <v>13.94790257104194</v>
       </c>
       <c r="B68" t="s">
         <v>51</v>
@@ -2153,12 +2154,12 @@
         <v>12</v>
       </c>
       <c r="E68">
-        <v>746</v>
+        <v>739</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B69" t="s">
         <v>52</v>
@@ -2170,12 +2171,12 @@
         <v>17</v>
       </c>
       <c r="E69">
-        <v>1553</v>
+        <v>1546</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B70" t="s">
         <v>52</v>
@@ -2187,12 +2188,12 @@
         <v>0</v>
       </c>
       <c r="E70">
-        <v>589</v>
+        <v>587</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B71" t="s">
         <v>53</v>
@@ -2204,12 +2205,12 @@
         <v>1</v>
       </c>
       <c r="E71">
-        <v>588</v>
+        <v>586</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B72" t="s">
         <v>53</v>
@@ -2221,12 +2222,12 @@
         <v>26</v>
       </c>
       <c r="E72">
-        <v>1534</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1521</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73">
-        <v>63.286096256684488</v>
+        <v>63.064777327935218</v>
       </c>
       <c r="B73" t="s">
         <v>53</v>
@@ -2238,12 +2239,12 @@
         <v>10</v>
       </c>
       <c r="E73">
-        <v>748</v>
+        <v>741</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B74" t="s">
         <v>54</v>
@@ -2255,12 +2256,12 @@
         <v>0</v>
       </c>
       <c r="E74">
-        <v>589</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75">
-        <v>43.321681538036977</v>
+        <v>42.714285714285687</v>
       </c>
       <c r="B75" t="s">
         <v>54</v>
@@ -2272,12 +2273,12 @@
         <v>7</v>
       </c>
       <c r="E75">
-        <v>1553</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1540</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76">
-        <v>101.71957671957669</v>
+        <v>101.4953271028037</v>
       </c>
       <c r="B76" t="s">
         <v>54</v>
@@ -2289,12 +2290,12 @@
         <v>2</v>
       </c>
       <c r="E76">
-        <v>756</v>
+        <v>749</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B77" t="s">
         <v>55</v>
@@ -2306,12 +2307,12 @@
         <v>0</v>
       </c>
       <c r="E77">
-        <v>589</v>
+        <v>587</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B78" t="s">
         <v>55</v>
@@ -2323,12 +2324,12 @@
         <v>8</v>
       </c>
       <c r="E78">
-        <v>1552</v>
+        <v>1539</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B79" t="s">
         <v>56</v>
@@ -2340,12 +2341,12 @@
         <v>0</v>
       </c>
       <c r="E79">
-        <v>589</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80">
-        <v>39.04942965779469</v>
+        <v>36.627906976744207</v>
       </c>
       <c r="B80" t="s">
         <v>56</v>
@@ -2357,12 +2358,12 @@
         <v>2</v>
       </c>
       <c r="E80">
-        <v>263</v>
+        <v>258</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B81" t="s">
         <v>57</v>
@@ -2374,12 +2375,12 @@
         <v>0</v>
       </c>
       <c r="E81">
-        <v>589</v>
+        <v>587</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B82" t="s">
         <v>57</v>
@@ -2396,7 +2397,7 @@
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B83" t="s">
         <v>57</v>
@@ -2408,12 +2409,12 @@
         <v>1</v>
       </c>
       <c r="E83">
-        <v>757</v>
+        <v>750</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B84" t="s">
         <v>58</v>
@@ -2425,12 +2426,12 @@
         <v>0</v>
       </c>
       <c r="E84">
-        <v>589</v>
+        <v>587</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B85" t="s">
         <v>58</v>
@@ -2447,7 +2448,7 @@
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B86" t="s">
         <v>58</v>
@@ -2459,12 +2460,12 @@
         <v>3</v>
       </c>
       <c r="E86">
-        <v>755</v>
+        <v>748</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B87" t="s">
         <v>59</v>
@@ -2476,12 +2477,12 @@
         <v>0</v>
       </c>
       <c r="E87">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B88" t="s">
         <v>59</v>
@@ -2493,12 +2494,12 @@
         <v>0</v>
       </c>
       <c r="E88">
-        <v>589</v>
+        <v>587</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B89" t="s">
         <v>61</v>
@@ -2510,12 +2511,12 @@
         <v>0</v>
       </c>
       <c r="E89">
-        <v>589</v>
+        <v>587</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B90" t="s">
         <v>61</v>
@@ -2527,12 +2528,12 @@
         <v>1</v>
       </c>
       <c r="E90">
-        <v>757</v>
+        <v>750</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B91" t="s">
         <v>62</v>
@@ -2544,12 +2545,12 @@
         <v>0</v>
       </c>
       <c r="E91">
-        <v>589</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92">
-        <v>39.430003623626021</v>
+        <v>39.102850212249848</v>
       </c>
       <c r="B92" t="s">
         <v>62</v>
@@ -2561,12 +2562,12 @@
         <v>34</v>
       </c>
       <c r="E92">
-        <v>2435</v>
+        <v>2425</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B93" t="s">
         <v>64</v>
@@ -2583,7 +2584,7 @@
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B94" t="s">
         <v>66</v>
@@ -2600,7 +2601,7 @@
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B95" t="s">
         <v>67</v>
@@ -2615,7 +2616,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>223.6363636363636</v>
       </c>
@@ -2634,7 +2635,7 @@
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B97" t="s">
         <v>69</v>
@@ -2651,7 +2652,7 @@
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B98" t="s">
         <v>70</v>
@@ -2668,7 +2669,7 @@
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B99" t="s">
         <v>71</v>
@@ -2685,7 +2686,7 @@
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B100" t="s">
         <v>72</v>
@@ -2702,7 +2703,7 @@
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B101" t="s">
         <v>73</v>
@@ -2719,7 +2720,7 @@
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B102" t="s">
         <v>74</v>
@@ -2736,7 +2737,7 @@
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B103" t="s">
         <v>75</v>
@@ -2753,7 +2754,7 @@
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B104" t="s">
         <v>76</v>
@@ -2770,7 +2771,7 @@
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B105" t="s">
         <v>77</v>
@@ -2787,7 +2788,7 @@
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B106" t="s">
         <v>78</v>
@@ -2804,7 +2805,7 @@
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B107" t="s">
         <v>79</v>
@@ -2821,7 +2822,7 @@
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B108" t="s">
         <v>80</v>
@@ -2838,7 +2839,7 @@
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B109" t="s">
         <v>81</v>
@@ -2855,7 +2856,7 @@
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B110" t="s">
         <v>82</v>
@@ -2867,12 +2868,12 @@
         <v>0</v>
       </c>
       <c r="E110">
-        <v>3014</v>
+        <v>2990</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B111" t="s">
         <v>82</v>
@@ -2884,12 +2885,12 @@
         <v>0</v>
       </c>
       <c r="E111">
-        <v>1560</v>
+        <v>1547</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B112" t="s">
         <v>82</v>
@@ -2901,12 +2902,12 @@
         <v>0</v>
       </c>
       <c r="E112">
-        <v>3015</v>
+        <v>2991</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B113" t="s">
         <v>82</v>
@@ -2918,12 +2919,12 @@
         <v>0</v>
       </c>
       <c r="E113">
-        <v>3453</v>
+        <v>3426</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B114" t="s">
         <v>82</v>
@@ -2940,7 +2941,7 @@
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B115" t="s">
         <v>85</v>
@@ -2957,7 +2958,7 @@
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B116" t="s">
         <v>86</v>
@@ -2974,7 +2975,7 @@
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B117" t="s">
         <v>87</v>
@@ -2991,7 +2992,7 @@
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B118" t="s">
         <v>87</v>
@@ -3003,12 +3004,12 @@
         <v>0</v>
       </c>
       <c r="E118">
-        <v>421</v>
+        <v>416</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B119" t="s">
         <v>87</v>
@@ -3025,7 +3026,7 @@
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B120" t="s">
         <v>90</v>
@@ -3042,7 +3043,7 @@
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B121" t="s">
         <v>90</v>
@@ -3057,7 +3058,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>46</v>
       </c>
@@ -3076,7 +3077,7 @@
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B123" t="s">
         <v>93</v>
@@ -3093,7 +3094,7 @@
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B124" t="s">
         <v>94</v>
@@ -3110,7 +3111,7 @@
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B125" t="s">
         <v>95</v>
@@ -3127,7 +3128,7 @@
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B126" t="s">
         <v>96</v>
@@ -3144,7 +3145,7 @@
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B127" t="s">
         <v>97</v>
@@ -3161,7 +3162,7 @@
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B128" t="s">
         <v>98</v>
@@ -3178,7 +3179,7 @@
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B129" t="s">
         <v>99</v>
@@ -3193,7 +3194,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>113.56321839080459</v>
       </c>
@@ -3212,7 +3213,7 @@
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B131" t="s">
         <v>101</v>
@@ -3229,7 +3230,7 @@
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B132" t="s">
         <v>102</v>
@@ -3241,12 +3242,12 @@
         <v>0</v>
       </c>
       <c r="E132">
-        <v>3014</v>
+        <v>2990</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B133" t="s">
         <v>102</v>
@@ -3258,12 +3259,12 @@
         <v>0</v>
       </c>
       <c r="E133">
-        <v>1560</v>
+        <v>1547</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A134">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B134" t="s">
         <v>102</v>
@@ -3280,7 +3281,7 @@
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A135">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B135" t="s">
         <v>103</v>
@@ -3292,12 +3293,12 @@
         <v>0</v>
       </c>
       <c r="E135">
-        <v>3014</v>
+        <v>2990</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B136" t="s">
         <v>103</v>
@@ -3309,12 +3310,12 @@
         <v>0</v>
       </c>
       <c r="E136">
-        <v>1560</v>
+        <v>1547</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B137" t="s">
         <v>103</v>
@@ -3331,7 +3332,7 @@
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A138">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B138" t="s">
         <v>104</v>
@@ -3348,7 +3349,7 @@
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A139">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B139" t="s">
         <v>105</v>
@@ -3365,7 +3366,7 @@
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A140">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B140" t="s">
         <v>106</v>
@@ -3382,7 +3383,7 @@
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B141" t="s">
         <v>107</v>
@@ -3394,12 +3395,12 @@
         <v>0</v>
       </c>
       <c r="E141">
-        <v>421</v>
+        <v>416</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B142" t="s">
         <v>107</v>
@@ -3416,7 +3417,7 @@
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A143">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B143" t="s">
         <v>108</v>
@@ -3433,7 +3434,7 @@
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A144">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B144" t="s">
         <v>109</v>
@@ -3450,7 +3451,7 @@
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A145">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B145" t="s">
         <v>110</v>
@@ -3467,7 +3468,7 @@
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A146">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B146" t="s">
         <v>111</v>
@@ -3484,7 +3485,7 @@
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A147">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B147" t="s">
         <v>112</v>
@@ -3499,9 +3500,9 @@
         <v>32</v>
       </c>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A148">
-        <v>10.454545454545441</v>
+        <v>14.244186046511629</v>
       </c>
       <c r="B148" t="s">
         <v>113</v>
@@ -3513,12 +3514,12 @@
         <v>8</v>
       </c>
       <c r="E148">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A149">
-        <v>12.217267009719849</v>
+        <v>11.873393491933291</v>
       </c>
       <c r="B149" t="s">
         <v>114</v>
@@ -3530,12 +3531,12 @@
         <v>159</v>
       </c>
       <c r="E149">
-        <v>2310</v>
+        <v>2300</v>
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A150">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B150" t="s">
         <v>114</v>
@@ -3547,12 +3548,12 @@
         <v>36</v>
       </c>
       <c r="E150">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A151">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B151" t="s">
         <v>116</v>
@@ -3564,12 +3565,12 @@
         <v>7</v>
       </c>
       <c r="E151">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A152">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B152" t="s">
         <v>117</v>
@@ -3581,12 +3582,12 @@
         <v>20</v>
       </c>
       <c r="E152">
-        <v>738</v>
-      </c>
-    </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A153">
-        <v>123.3333333333333</v>
+        <v>126.968085106383</v>
       </c>
       <c r="B153" t="s">
         <v>117</v>
@@ -3598,12 +3599,12 @@
         <v>4</v>
       </c>
       <c r="E153">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A154">
-        <v>18.482358558671219</v>
+        <v>17.89734890868559</v>
       </c>
       <c r="B154" t="s">
         <v>118</v>
@@ -3612,15 +3613,15 @@
         <v>63</v>
       </c>
       <c r="D154">
-        <v>893</v>
+        <v>892</v>
       </c>
       <c r="E154">
-        <v>1576</v>
+        <v>1567</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A155">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B155" t="s">
         <v>119</v>
@@ -3632,12 +3633,12 @@
         <v>27</v>
       </c>
       <c r="E155">
-        <v>562</v>
-      </c>
-    </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A156">
-        <v>47.359117270467721</v>
+        <v>47.031235819089403</v>
       </c>
       <c r="B156" t="s">
         <v>119</v>
@@ -3649,12 +3650,12 @@
         <v>55</v>
       </c>
       <c r="E156">
-        <v>2414</v>
+        <v>2404</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A157">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B157" t="s">
         <v>120</v>
@@ -3663,15 +3664,15 @@
         <v>121</v>
       </c>
       <c r="D157">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E157">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A158">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B158" t="s">
         <v>120</v>
@@ -3680,15 +3681,15 @@
         <v>122</v>
       </c>
       <c r="D158">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E158">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A159">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B159" t="s">
         <v>120</v>
@@ -3703,9 +3704,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A160">
-        <v>10.11154805773484</v>
+        <v>9.7217330199528931</v>
       </c>
       <c r="B160" t="s">
         <v>123</v>
@@ -3717,12 +3718,12 @@
         <v>458</v>
       </c>
       <c r="E160">
-        <v>2011</v>
-      </c>
-    </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A161">
-        <v>24.883245893179691</v>
+        <v>24.65803041179927</v>
       </c>
       <c r="B161" t="s">
         <v>123</v>
@@ -3734,12 +3735,12 @@
         <v>154</v>
       </c>
       <c r="E161">
-        <v>604</v>
+        <v>597</v>
       </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A162">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B162" t="s">
         <v>124</v>
@@ -3756,7 +3757,7 @@
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A163">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B163" t="s">
         <v>124</v>
@@ -3768,12 +3769,12 @@
         <v>1</v>
       </c>
       <c r="E163">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A164">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B164" t="s">
         <v>125</v>
@@ -3785,12 +3786,12 @@
         <v>9</v>
       </c>
       <c r="E164">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A165">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B165" t="s">
         <v>125</v>
@@ -3802,12 +3803,12 @@
         <v>91</v>
       </c>
       <c r="E165">
-        <v>1479</v>
+        <v>1472</v>
       </c>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A166">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B166" t="s">
         <v>126</v>
@@ -3816,15 +3817,15 @@
         <v>39</v>
       </c>
       <c r="D166">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E166">
         <v>232</v>
       </c>
     </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A167">
-        <v>3.6882696840355318</v>
+        <v>3.907989282669575</v>
       </c>
       <c r="B167" t="s">
         <v>126</v>
@@ -3833,15 +3834,15 @@
         <v>63</v>
       </c>
       <c r="D167">
-        <v>508</v>
+        <v>504</v>
       </c>
       <c r="E167">
-        <v>1961</v>
+        <v>1955</v>
       </c>
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A168">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B168" t="s">
         <v>127</v>
@@ -3853,12 +3854,12 @@
         <v>156</v>
       </c>
       <c r="E168">
-        <v>1414</v>
+        <v>1407</v>
       </c>
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A169">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B169" t="s">
         <v>127</v>
@@ -3870,12 +3871,12 @@
         <v>26</v>
       </c>
       <c r="E169">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A170">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B170" t="s">
         <v>127</v>
@@ -3887,12 +3888,12 @@
         <v>28</v>
       </c>
       <c r="E170">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A171">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B171" t="s">
         <v>128</v>
@@ -3904,12 +3905,12 @@
         <v>0</v>
       </c>
       <c r="E171">
-        <v>234</v>
+        <v>229</v>
       </c>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A172">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B172" t="s">
         <v>128</v>
@@ -3926,7 +3927,7 @@
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A173">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B173" t="s">
         <v>128</v>
@@ -3938,12 +3939,12 @@
         <v>0</v>
       </c>
       <c r="E173">
-        <v>758</v>
+        <v>751</v>
       </c>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A174">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B174" t="s">
         <v>129</v>
@@ -3952,15 +3953,15 @@
         <v>6</v>
       </c>
       <c r="D174">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E174">
-        <v>1414</v>
+        <v>1408</v>
       </c>
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A175">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B175" t="s">
         <v>129</v>
@@ -3972,12 +3973,12 @@
         <v>59</v>
       </c>
       <c r="E175">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A176">
-        <v>25.182664756447</v>
+        <v>24.738372093023258</v>
       </c>
       <c r="B176" t="s">
         <v>129</v>
@@ -3989,12 +3990,12 @@
         <v>72</v>
       </c>
       <c r="E176">
-        <v>349</v>
+        <v>344</v>
       </c>
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A177">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B177" t="s">
         <v>129</v>
@@ -4003,15 +4004,15 @@
         <v>130</v>
       </c>
       <c r="D177">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E177">
-        <v>610</v>
-      </c>
-    </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="178" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A178">
-        <v>39.430003623626021</v>
+        <v>39.102850212249848</v>
       </c>
       <c r="B178" t="s">
         <v>131</v>
@@ -4023,12 +4024,12 @@
         <v>34</v>
       </c>
       <c r="E178">
-        <v>2435</v>
+        <v>2425</v>
       </c>
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A179">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B179" t="s">
         <v>131</v>
@@ -4040,12 +4041,12 @@
         <v>0</v>
       </c>
       <c r="E179">
-        <v>589</v>
+        <v>587</v>
       </c>
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A180">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B180" t="s">
         <v>132</v>
@@ -4057,12 +4058,12 @@
         <v>0</v>
       </c>
       <c r="E180">
-        <v>589</v>
-      </c>
-    </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="181" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A181">
-        <v>25.47</v>
+        <v>25.243943472409139</v>
       </c>
       <c r="B181" t="s">
         <v>132</v>
@@ -4074,12 +4075,12 @@
         <v>8</v>
       </c>
       <c r="E181">
-        <v>750</v>
-      </c>
-    </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="182" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A182">
-        <v>127.1861471861472</v>
+        <v>124.7492625368731</v>
       </c>
       <c r="B182" t="s">
         <v>132</v>
@@ -4091,12 +4092,12 @@
         <v>3</v>
       </c>
       <c r="E182">
-        <v>231</v>
+        <v>226</v>
       </c>
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A183">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B183" t="s">
         <v>132</v>
@@ -4113,7 +4114,7 @@
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A184">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B184" t="s">
         <v>133</v>
@@ -4125,12 +4126,12 @@
         <v>0</v>
       </c>
       <c r="E184">
-        <v>589</v>
-      </c>
-    </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="185" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A185">
-        <v>28.03565715098296</v>
+        <v>27.70882415934889</v>
       </c>
       <c r="B185" t="s">
         <v>133</v>
@@ -4142,12 +4143,12 @@
         <v>23</v>
       </c>
       <c r="E185">
-        <v>2446</v>
+        <v>2436</v>
       </c>
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A186">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B186" t="s">
         <v>134</v>
@@ -4159,12 +4160,12 @@
         <v>0</v>
       </c>
       <c r="E186">
-        <v>589</v>
-      </c>
-    </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="187" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A187">
-        <v>42.139384116693691</v>
+        <v>41.814483319772172</v>
       </c>
       <c r="B187" t="s">
         <v>134</v>
@@ -4176,12 +4177,12 @@
         <v>1</v>
       </c>
       <c r="E187">
-        <v>2468</v>
+        <v>2458</v>
       </c>
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A188">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B188" t="s">
         <v>134</v>
@@ -4193,12 +4194,12 @@
         <v>0</v>
       </c>
       <c r="E188">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="189" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A189">
-        <v>24.78468899521533</v>
+        <v>24.358560221504401</v>
       </c>
       <c r="B189" t="s">
         <v>135</v>
@@ -4210,12 +4211,12 @@
         <v>22</v>
       </c>
       <c r="E189">
-        <v>399</v>
+        <v>394</v>
       </c>
     </row>
     <row r="190" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A190">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B190" t="s">
         <v>136</v>
@@ -4227,12 +4228,12 @@
         <v>12</v>
       </c>
       <c r="E190">
-        <v>409</v>
+        <v>404</v>
       </c>
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A191">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B191" t="s">
         <v>137</v>
@@ -4244,12 +4245,12 @@
         <v>11</v>
       </c>
       <c r="E191">
-        <v>410</v>
+        <v>405</v>
       </c>
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A192">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B192" t="s">
         <v>138</v>
@@ -4261,12 +4262,12 @@
         <v>11</v>
       </c>
       <c r="E192">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="193" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A193">
-        <v>77.865707434052752</v>
+        <v>77.451456310679617</v>
       </c>
       <c r="B193" t="s">
         <v>139</v>
@@ -4278,12 +4279,12 @@
         <v>4</v>
       </c>
       <c r="E193">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="194" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A194">
-        <v>122.708830548926</v>
+        <v>122.29468599033819</v>
       </c>
       <c r="B194" t="s">
         <v>140</v>
@@ -4295,12 +4296,12 @@
         <v>2</v>
       </c>
       <c r="E194">
-        <v>419</v>
+        <v>414</v>
       </c>
     </row>
     <row r="195" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A195">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B195" t="s">
         <v>141</v>
@@ -4312,12 +4313,12 @@
         <v>0</v>
       </c>
       <c r="E195">
-        <v>421</v>
+        <v>416</v>
       </c>
     </row>
     <row r="196" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A196">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B196" t="s">
         <v>142</v>
@@ -4329,12 +4330,12 @@
         <v>64</v>
       </c>
       <c r="E196">
-        <v>357</v>
+        <v>352</v>
       </c>
     </row>
     <row r="197" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A197">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B197" t="s">
         <v>143</v>
@@ -4346,12 +4347,12 @@
         <v>4</v>
       </c>
       <c r="E197">
-        <v>417</v>
+        <v>412</v>
       </c>
     </row>
     <row r="198" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A198">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B198" t="s">
         <v>144</v>
@@ -4363,12 +4364,12 @@
         <v>28</v>
       </c>
       <c r="E198">
-        <v>2441</v>
+        <v>2431</v>
       </c>
     </row>
     <row r="199" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A199">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B199" t="s">
         <v>144</v>
@@ -4380,12 +4381,12 @@
         <v>10</v>
       </c>
       <c r="E199">
-        <v>411</v>
+        <v>406</v>
       </c>
     </row>
     <row r="200" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A200">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B200" t="s">
         <v>145</v>
@@ -4397,12 +4398,12 @@
         <v>5</v>
       </c>
       <c r="E200">
-        <v>416</v>
+        <v>411</v>
       </c>
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A201">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B201" t="s">
         <v>146</v>
@@ -4414,12 +4415,12 @@
         <v>0</v>
       </c>
       <c r="E201">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="202" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A202">
-        <v>137.45238095238099</v>
+        <v>137.03614457831321</v>
       </c>
       <c r="B202" t="s">
         <v>147</v>
@@ -4431,12 +4432,12 @@
         <v>1</v>
       </c>
       <c r="E202">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="203" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A203">
-        <v>37.214285714285722</v>
+        <v>36.795180722891558</v>
       </c>
       <c r="B203" t="s">
         <v>148</v>
@@ -4448,12 +4449,12 @@
         <v>1</v>
       </c>
       <c r="E203">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="204" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A204">
-        <v>67.285714285714278</v>
+        <v>66.867469879518069</v>
       </c>
       <c r="B204" t="s">
         <v>149</v>
@@ -4465,12 +4466,12 @@
         <v>1</v>
       </c>
       <c r="E204">
-        <v>420</v>
+        <v>415</v>
       </c>
     </row>
     <row r="205" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A205">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B205" t="s">
         <v>150</v>
@@ -4482,12 +4483,12 @@
         <v>5</v>
       </c>
       <c r="E205">
-        <v>416</v>
+        <v>411</v>
       </c>
     </row>
     <row r="206" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A206">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B206" t="s">
         <v>151</v>
@@ -4499,12 +4500,12 @@
         <v>0</v>
       </c>
       <c r="E206">
-        <v>421</v>
+        <v>416</v>
       </c>
     </row>
     <row r="207" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A207">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B207" t="s">
         <v>152</v>
@@ -4516,12 +4517,12 @@
         <v>0</v>
       </c>
       <c r="E207">
-        <v>421</v>
+        <v>416</v>
       </c>
     </row>
     <row r="208" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A208">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B208" t="s">
         <v>153</v>
@@ -4533,12 +4534,12 @@
         <v>0</v>
       </c>
       <c r="E208">
-        <v>589</v>
+        <v>587</v>
       </c>
     </row>
     <row r="209" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A209">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B209" t="s">
         <v>153</v>
@@ -4550,12 +4551,12 @@
         <v>0</v>
       </c>
       <c r="E209">
-        <v>421</v>
+        <v>416</v>
       </c>
     </row>
     <row r="210" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A210">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B210" t="s">
         <v>154</v>
@@ -4567,12 +4568,12 @@
         <v>0</v>
       </c>
       <c r="E210">
-        <v>421</v>
+        <v>416</v>
       </c>
     </row>
     <row r="211" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A211">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B211" t="s">
         <v>155</v>
@@ -4584,12 +4585,12 @@
         <v>0</v>
       </c>
       <c r="E211">
-        <v>589</v>
+        <v>587</v>
       </c>
     </row>
     <row r="212" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A212">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B212" t="s">
         <v>155</v>
@@ -4601,12 +4602,12 @@
         <v>0</v>
       </c>
       <c r="E212">
-        <v>421</v>
+        <v>416</v>
       </c>
     </row>
     <row r="213" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A213">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B213" t="s">
         <v>156</v>
@@ -4618,12 +4619,12 @@
         <v>0</v>
       </c>
       <c r="E213">
-        <v>589</v>
-      </c>
-    </row>
-    <row r="214" spans="1:5" x14ac:dyDescent="0.25">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="214" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A214">
-        <v>107.38095238095239</v>
+        <v>106.9638554216868</v>
       </c>
       <c r="B214" t="s">
         <v>156</v>
@@ -4635,12 +4636,12 @@
         <v>1</v>
       </c>
       <c r="E214">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="215" spans="1:5" x14ac:dyDescent="0.25">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="215" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A215">
-        <v>78.863247863247864</v>
+        <v>79.065180102915946</v>
       </c>
       <c r="B215" t="s">
         <v>157</v>
@@ -4652,12 +4653,12 @@
         <v>4</v>
       </c>
       <c r="E215">
-        <v>585</v>
+        <v>583</v>
       </c>
     </row>
     <row r="216" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A216">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B216" t="s">
         <v>157</v>
@@ -4669,12 +4670,12 @@
         <v>0</v>
       </c>
       <c r="E216">
-        <v>421</v>
+        <v>416</v>
       </c>
     </row>
     <row r="217" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A217">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B217" t="s">
         <v>158</v>
@@ -4686,12 +4687,12 @@
         <v>0</v>
       </c>
       <c r="E217">
-        <v>589</v>
+        <v>587</v>
       </c>
     </row>
     <row r="218" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A218">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B218" t="s">
         <v>158</v>
@@ -4703,12 +4704,12 @@
         <v>0</v>
       </c>
       <c r="E218">
-        <v>421</v>
+        <v>416</v>
       </c>
     </row>
     <row r="219" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A219">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B219" t="s">
         <v>159</v>
@@ -4720,12 +4721,12 @@
         <v>8</v>
       </c>
       <c r="E219">
-        <v>413</v>
+        <v>408</v>
       </c>
     </row>
     <row r="220" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A220">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B220" t="s">
         <v>160</v>
@@ -4737,12 +4738,12 @@
         <v>0</v>
       </c>
       <c r="E220">
-        <v>421</v>
+        <v>416</v>
       </c>
     </row>
     <row r="221" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A221">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B221" t="s">
         <v>161</v>
@@ -4754,12 +4755,12 @@
         <v>0</v>
       </c>
       <c r="E221">
-        <v>421</v>
+        <v>416</v>
       </c>
     </row>
     <row r="222" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A222">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B222" t="s">
         <v>162</v>
@@ -4776,7 +4777,7 @@
     </row>
     <row r="223" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A223">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B223" t="s">
         <v>162</v>
@@ -4788,12 +4789,12 @@
         <v>0</v>
       </c>
       <c r="E223">
-        <v>421</v>
+        <v>416</v>
       </c>
     </row>
     <row r="224" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A224">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B224" t="s">
         <v>163</v>
@@ -4805,12 +4806,12 @@
         <v>0</v>
       </c>
       <c r="E224">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="225" spans="1:5" x14ac:dyDescent="0.25">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="225" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A225">
-        <v>35.351517479830932</v>
+        <v>35.437567525852728</v>
       </c>
       <c r="B225" t="s">
         <v>164</v>
@@ -4822,12 +4823,12 @@
         <v>38</v>
       </c>
       <c r="E225">
-        <v>685</v>
+        <v>682</v>
       </c>
     </row>
     <row r="226" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A226">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B226" t="s">
         <v>165</v>
@@ -4839,12 +4840,12 @@
         <v>21</v>
       </c>
       <c r="E226">
-        <v>737</v>
+        <v>730</v>
       </c>
     </row>
     <row r="227" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A227">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B227" t="s">
         <v>165</v>
@@ -4856,12 +4857,12 @@
         <v>40</v>
       </c>
       <c r="E227">
-        <v>3413</v>
-      </c>
-    </row>
-    <row r="228" spans="1:5" x14ac:dyDescent="0.25">
+        <v>3386</v>
+      </c>
+    </row>
+    <row r="228" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A228">
-        <v>32.885952712100163</v>
+        <v>32.960893854748583</v>
       </c>
       <c r="B228" t="s">
         <v>165</v>
@@ -4873,12 +4874,12 @@
         <v>4</v>
       </c>
       <c r="E228">
-        <v>719</v>
+        <v>716</v>
       </c>
     </row>
     <row r="229" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A229">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B229" t="s">
         <v>166</v>
@@ -4887,15 +4888,15 @@
         <v>14</v>
       </c>
       <c r="D229">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E229">
-        <v>3323</v>
+        <v>3297</v>
       </c>
     </row>
     <row r="230" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A230">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B230" t="s">
         <v>166</v>
@@ -4907,12 +4908,12 @@
         <v>20</v>
       </c>
       <c r="E230">
-        <v>703</v>
+        <v>700</v>
       </c>
     </row>
     <row r="231" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A231">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B231" t="s">
         <v>167</v>
@@ -4924,12 +4925,12 @@
         <v>22</v>
       </c>
       <c r="E231">
-        <v>701</v>
+        <v>698</v>
       </c>
     </row>
     <row r="232" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A232">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B232" t="s">
         <v>168</v>
@@ -4941,12 +4942,12 @@
         <v>34</v>
       </c>
       <c r="E232">
-        <v>689</v>
-      </c>
-    </row>
-    <row r="233" spans="1:5" x14ac:dyDescent="0.25">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="233" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A233">
-        <v>18.722338516746451</v>
+        <v>18.800210225992942</v>
       </c>
       <c r="B233" t="s">
         <v>169</v>
@@ -4958,12 +4959,12 @@
         <v>19</v>
       </c>
       <c r="E233">
-        <v>704</v>
+        <v>701</v>
       </c>
     </row>
     <row r="234" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A234">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B234" t="s">
         <v>170</v>
@@ -4975,12 +4976,12 @@
         <v>0</v>
       </c>
       <c r="E234">
-        <v>723</v>
-      </c>
-    </row>
-    <row r="235" spans="1:5" x14ac:dyDescent="0.25">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="235" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A235">
-        <v>90.705841446453405</v>
+        <v>90.782122905027961</v>
       </c>
       <c r="B235" t="s">
         <v>171</v>
@@ -4992,12 +4993,12 @@
         <v>4</v>
       </c>
       <c r="E235">
-        <v>719</v>
-      </c>
-    </row>
-    <row r="236" spans="1:5" x14ac:dyDescent="0.25">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="236" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A236">
-        <v>21.69405594405595</v>
+        <v>21.769662921348299</v>
       </c>
       <c r="B236" t="s">
         <v>172</v>
@@ -5009,12 +5010,12 @@
         <v>8</v>
       </c>
       <c r="E236">
-        <v>715</v>
+        <v>712</v>
       </c>
     </row>
     <row r="237" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A237">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B237" t="s">
         <v>173</v>
@@ -5026,12 +5027,12 @@
         <v>32</v>
       </c>
       <c r="E237">
-        <v>691</v>
+        <v>688</v>
       </c>
     </row>
     <row r="238" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A238">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B238" t="s">
         <v>174</v>
@@ -5043,12 +5044,12 @@
         <v>3</v>
       </c>
       <c r="E238">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="239" spans="1:5" x14ac:dyDescent="0.25">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="239" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A239">
-        <v>143.0998613037448</v>
+        <v>143.17548746518099</v>
       </c>
       <c r="B239" t="s">
         <v>174</v>
@@ -5060,12 +5061,12 @@
         <v>2</v>
       </c>
       <c r="E239">
-        <v>721</v>
-      </c>
-    </row>
-    <row r="240" spans="1:5" x14ac:dyDescent="0.25">
+        <v>718</v>
+      </c>
+    </row>
+    <row r="240" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A240">
-        <v>0.7952329360780368</v>
+        <v>0.87041671200086057</v>
       </c>
       <c r="B240" t="s">
         <v>175</v>
@@ -5077,12 +5078,12 @@
         <v>13</v>
       </c>
       <c r="E240">
-        <v>710</v>
+        <v>707</v>
       </c>
     </row>
     <row r="241" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A241">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B241" t="s">
         <v>176</v>
@@ -5094,12 +5095,12 @@
         <v>0</v>
       </c>
       <c r="E241">
-        <v>723</v>
-      </c>
-    </row>
-    <row r="242" spans="1:5" x14ac:dyDescent="0.25">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="242" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A242">
-        <v>62.133704735376057</v>
+        <v>62.209790209790192</v>
       </c>
       <c r="B242" t="s">
         <v>177</v>
@@ -5111,12 +5112,12 @@
         <v>5</v>
       </c>
       <c r="E242">
-        <v>718</v>
-      </c>
-    </row>
-    <row r="243" spans="1:5" x14ac:dyDescent="0.25">
+        <v>715</v>
+      </c>
+    </row>
+    <row r="243" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A243">
-        <v>137.89473684210529</v>
+        <v>137.96940194714881</v>
       </c>
       <c r="B243" t="s">
         <v>178</v>
@@ -5128,12 +5129,12 @@
         <v>1</v>
       </c>
       <c r="E243">
-        <v>722</v>
+        <v>719</v>
       </c>
     </row>
     <row r="244" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A244">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B244" t="s">
         <v>179</v>
@@ -5145,12 +5146,12 @@
         <v>9</v>
       </c>
       <c r="E244">
-        <v>714</v>
-      </c>
-    </row>
-    <row r="245" spans="1:5" x14ac:dyDescent="0.25">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="245" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A245">
-        <v>9.8221206399682046</v>
+        <v>12.551610239471531</v>
       </c>
       <c r="B245" t="s">
         <v>180</v>
@@ -5159,15 +5160,15 @@
         <v>130</v>
       </c>
       <c r="D245">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E245">
-        <v>694</v>
-      </c>
-    </row>
-    <row r="246" spans="1:5" x14ac:dyDescent="0.25">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="246" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A246">
-        <v>7.7146814404432007</v>
+        <v>7.7885952712099993</v>
       </c>
       <c r="B246" t="s">
         <v>181</v>
@@ -5179,12 +5180,12 @@
         <v>1</v>
       </c>
       <c r="E246">
-        <v>722</v>
-      </c>
-    </row>
-    <row r="247" spans="1:5" x14ac:dyDescent="0.25">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="247" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A247">
-        <v>32.931792488380893</v>
+        <v>32.627783400809733</v>
       </c>
       <c r="B247" t="s">
         <v>182</v>
@@ -5196,12 +5197,12 @@
         <v>19</v>
       </c>
       <c r="E247">
-        <v>419</v>
+        <v>416</v>
       </c>
     </row>
     <row r="248" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A248">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B248" t="s">
         <v>184</v>
@@ -5213,12 +5214,12 @@
         <v>16</v>
       </c>
       <c r="E248">
-        <v>707</v>
-      </c>
-    </row>
-    <row r="249" spans="1:5" x14ac:dyDescent="0.25">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="249" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A249">
-        <v>8.9928229665071626</v>
+        <v>8.6807228915662904</v>
       </c>
       <c r="B249" t="s">
         <v>184</v>
@@ -5230,12 +5231,12 @@
         <v>20</v>
       </c>
       <c r="E249">
-        <v>418</v>
+        <v>415</v>
       </c>
     </row>
     <row r="250" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A250">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B250" t="s">
         <v>185</v>
@@ -5247,12 +5248,12 @@
         <v>0</v>
       </c>
       <c r="E250">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="251" spans="1:5" x14ac:dyDescent="0.25">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="251" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A251">
-        <v>27.39491916859123</v>
+        <v>27.093023255813929</v>
       </c>
       <c r="B251" t="s">
         <v>186</v>
@@ -5264,12 +5265,12 @@
         <v>5</v>
       </c>
       <c r="E251">
-        <v>433</v>
+        <v>430</v>
       </c>
     </row>
     <row r="252" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A252">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B252" t="s">
         <v>187</v>
@@ -5281,12 +5282,12 @@
         <v>0</v>
       </c>
       <c r="E252">
-        <v>438</v>
+        <v>435</v>
       </c>
     </row>
     <row r="253" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A253">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B253" t="s">
         <v>188</v>
@@ -5298,12 +5299,12 @@
         <v>2</v>
       </c>
       <c r="E253">
-        <v>2467</v>
+        <v>2457</v>
       </c>
     </row>
     <row r="254" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A254">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B254" t="s">
         <v>188</v>
@@ -5315,12 +5316,12 @@
         <v>6</v>
       </c>
       <c r="E254">
-        <v>432</v>
-      </c>
-    </row>
-    <row r="255" spans="1:5" x14ac:dyDescent="0.25">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="255" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A255">
-        <v>7.4736125297923186</v>
+        <v>7.1406501285314619</v>
       </c>
       <c r="B255" t="s">
         <v>189</v>
@@ -5332,12 +5333,12 @@
         <v>66</v>
       </c>
       <c r="E255">
-        <v>2403</v>
-      </c>
-    </row>
-    <row r="256" spans="1:5" x14ac:dyDescent="0.25">
+        <v>2393</v>
+      </c>
+    </row>
+    <row r="256" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A256">
-        <v>132.33617437473811</v>
+        <v>132.06023079088101</v>
       </c>
       <c r="B256" t="s">
         <v>189</v>
@@ -5349,12 +5350,12 @@
         <v>17</v>
       </c>
       <c r="E256">
-        <v>421</v>
+        <v>418</v>
       </c>
     </row>
     <row r="257" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A257">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B257" t="s">
         <v>190</v>
@@ -5366,12 +5367,12 @@
         <v>0</v>
       </c>
       <c r="E257">
-        <v>758</v>
+        <v>751</v>
       </c>
     </row>
     <row r="258" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A258">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B258" t="s">
         <v>190</v>
@@ -5383,12 +5384,12 @@
         <v>0</v>
       </c>
       <c r="E258">
-        <v>3014</v>
+        <v>2990</v>
       </c>
     </row>
     <row r="259" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A259">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B259" t="s">
         <v>190</v>
@@ -5400,12 +5401,12 @@
         <v>0</v>
       </c>
       <c r="E259">
-        <v>3015</v>
+        <v>2991</v>
       </c>
     </row>
     <row r="260" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A260">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B260" t="s">
         <v>190</v>
@@ -5417,12 +5418,12 @@
         <v>0</v>
       </c>
       <c r="E260">
-        <v>438</v>
+        <v>435</v>
       </c>
     </row>
     <row r="261" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A261">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B261" t="s">
         <v>191</v>
@@ -5434,12 +5435,12 @@
         <v>0</v>
       </c>
       <c r="E261">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="262" spans="1:5" x14ac:dyDescent="0.25">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="262" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A262">
-        <v>16.742034943473751</v>
+        <v>16.432022084195982</v>
       </c>
       <c r="B262" t="s">
         <v>192</v>
@@ -5451,12 +5452,12 @@
         <v>21</v>
       </c>
       <c r="E262">
-        <v>417</v>
+        <v>414</v>
       </c>
     </row>
     <row r="263" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A263">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B263" t="s">
         <v>193</v>
@@ -5468,12 +5469,12 @@
         <v>4</v>
       </c>
       <c r="E263">
-        <v>434</v>
+        <v>431</v>
       </c>
     </row>
     <row r="264" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A264">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B264" t="s">
         <v>194</v>
@@ -5485,12 +5486,12 @@
         <v>0</v>
       </c>
       <c r="E264">
-        <v>438</v>
+        <v>435</v>
       </c>
     </row>
     <row r="265" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A265">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B265" t="s">
         <v>195</v>
@@ -5502,12 +5503,12 @@
         <v>6</v>
       </c>
       <c r="E265">
-        <v>432</v>
-      </c>
-    </row>
-    <row r="266" spans="1:5" x14ac:dyDescent="0.25">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="266" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A266">
-        <v>103.31807780320371</v>
+        <v>103.0184331797235</v>
       </c>
       <c r="B266" t="s">
         <v>196</v>
@@ -5519,12 +5520,12 @@
         <v>1</v>
       </c>
       <c r="E266">
-        <v>437</v>
-      </c>
-    </row>
-    <row r="267" spans="1:5" x14ac:dyDescent="0.25">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="267" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A267">
-        <v>15.725806451612931</v>
+        <v>15.423433874709991</v>
       </c>
       <c r="B267" t="s">
         <v>197</v>
@@ -5536,12 +5537,12 @@
         <v>4</v>
       </c>
       <c r="E267">
-        <v>434</v>
+        <v>431</v>
       </c>
     </row>
     <row r="268" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A268">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B268" t="s">
         <v>198</v>
@@ -5553,12 +5554,12 @@
         <v>2</v>
       </c>
       <c r="E268">
-        <v>436</v>
+        <v>433</v>
       </c>
     </row>
     <row r="269" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A269">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B269" t="s">
         <v>199</v>
@@ -5570,12 +5571,12 @@
         <v>0</v>
       </c>
       <c r="E269">
-        <v>438</v>
+        <v>435</v>
       </c>
     </row>
     <row r="270" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A270">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B270" t="s">
         <v>200</v>
@@ -5587,12 +5588,12 @@
         <v>0</v>
       </c>
       <c r="E270">
-        <v>421</v>
+        <v>416</v>
       </c>
     </row>
     <row r="271" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A271">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B271" t="s">
         <v>200</v>
@@ -5604,12 +5605,12 @@
         <v>0</v>
       </c>
       <c r="E271">
-        <v>438</v>
+        <v>435</v>
       </c>
     </row>
     <row r="272" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A272">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B272" t="s">
         <v>201</v>
@@ -5621,12 +5622,12 @@
         <v>0</v>
       </c>
       <c r="E272">
-        <v>421</v>
+        <v>416</v>
       </c>
     </row>
     <row r="273" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A273">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B273" t="s">
         <v>201</v>
@@ -5638,11 +5639,17 @@
         <v>0</v>
       </c>
       <c r="E273">
-        <v>438</v>
+        <v>435</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E273" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:E273" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="0,001"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>